<commit_message>
Continuing the manuel : end of all caracs
</commit_message>
<xml_diff>
--- a/Autres/Equilibrage/Tableau_Dépendance_Stats.xlsx
+++ b/Autres/Equilibrage/Tableau_Dépendance_Stats.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="83">
   <si>
     <t>Stress</t>
   </si>
@@ -193,6 +193,90 @@
   </si>
   <si>
     <t>AttaqueZombi</t>
+  </si>
+  <si>
+    <t>Attribut 4</t>
+  </si>
+  <si>
+    <t>Poids 4</t>
+  </si>
+  <si>
+    <t>Poids 5</t>
+  </si>
+  <si>
+    <t>Attribut 5</t>
+  </si>
+  <si>
+    <t>ReactionSM</t>
+  </si>
+  <si>
+    <t>Max(5)</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>RelAmical</t>
+  </si>
+  <si>
+    <t>RelAmour</t>
+  </si>
+  <si>
+    <t>_1/2</t>
+  </si>
+  <si>
+    <t>Perte SM</t>
+  </si>
+  <si>
+    <t>Mort perso</t>
+  </si>
+  <si>
+    <t>Note : Max(X-Y) signifie qu'on cherche à maximiser la valeur pour obtenir un poids allant de X à Y.</t>
+  </si>
+  <si>
+    <t>Min(9-5)</t>
+  </si>
+  <si>
+    <t>Min(8-4)</t>
+  </si>
+  <si>
+    <t>Min(5-3)</t>
+  </si>
+  <si>
+    <t>(1/10)^-1</t>
+  </si>
+  <si>
+    <t>GainStress</t>
+  </si>
+  <si>
+    <t>_01/10</t>
+  </si>
+  <si>
+    <t>PerteStress</t>
+  </si>
+  <si>
+    <t>_10/3</t>
+  </si>
+  <si>
+    <t>(1/20)^-1</t>
+  </si>
+  <si>
+    <t>_+1</t>
+  </si>
+  <si>
+    <t>_+0,1</t>
+  </si>
+  <si>
+    <t>_+0,6</t>
+  </si>
+  <si>
+    <t>_+4</t>
+  </si>
+  <si>
+    <t>Bruit</t>
+  </si>
+  <si>
+    <t>_+2</t>
   </si>
 </sst>
 </file>
@@ -222,7 +306,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -232,6 +316,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -263,7 +353,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -277,52 +367,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -619,10 +680,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J38"/>
+  <dimension ref="A1:P41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H16" sqref="H1:H1048576"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -635,12 +696,18 @@
     <col min="6" max="6" width="13.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="2.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="11.42578125" style="2"/>
+    <col min="9" max="9" width="8.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="2.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="2.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -665,8 +732,22 @@
       <c r="J1" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" s="1"/>
+      <c r="L1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
@@ -685,8 +766,18 @@
       </c>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -711,10 +802,28 @@
       <c r="H3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I3" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L3" s="1">
+        <v>4</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
@@ -745,28 +854,48 @@
       <c r="J4" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="K4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="O5" s="7"/>
+      <c r="P5" s="7"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
@@ -782,35 +911,63 @@
       <c r="E6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
+      <c r="F6" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="H6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="I6" s="4">
+        <v>1</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="O7" s="7"/>
+      <c r="P7" s="7"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>2</v>
       </c>
@@ -833,132 +990,208 @@
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="K8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="B9" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="O9" s="8"/>
+      <c r="P9" s="8"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="B10" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="O10" s="8"/>
+      <c r="P10" s="8"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="1" t="s">
+      <c r="B11" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F11" s="1" t="s">
+      <c r="E11" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="G11" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="H11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="H11" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="K11" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="L11" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="M11" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="N11" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="O11" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="P11" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" s="1" t="s">
+      <c r="B12" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F12" s="1" t="s">
+      <c r="E12" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="G12" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="H12" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="H12" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="O12" s="7"/>
+      <c r="P12" s="7"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="O13" s="7"/>
+      <c r="P13" s="7"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
+      <c r="C14" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="E14" s="1" t="s">
         <v>7</v>
       </c>
@@ -969,148 +1202,288 @@
       </c>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
+      <c r="C15" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="E15" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
+      <c r="F15" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>72</v>
+      </c>
       <c r="H15" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I15" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
+      <c r="C16" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="E16" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
+      <c r="F16" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>66</v>
+      </c>
       <c r="H16" s="1" t="s">
         <v>7</v>
       </c>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
+      <c r="C17" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>62</v>
+      </c>
       <c r="E17" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
+      <c r="F17" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="H17" s="1" t="s">
         <v>7</v>
       </c>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="K17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="B18" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="L18" s="7"/>
+      <c r="M18" s="7"/>
+      <c r="N18" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="O18" s="7"/>
+      <c r="P18" s="7"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+      <c r="B19" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="L19" s="7"/>
+      <c r="M19" s="7"/>
+      <c r="N19" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="O19" s="7"/>
+      <c r="P19" s="7"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="B20" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="H20" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I20" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="J20" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K20" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="O20" s="7"/>
+      <c r="P20" s="7"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B21" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H21" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I21" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="J21" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="K21" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="L21" s="7"/>
+      <c r="M21" s="7"/>
+      <c r="N21" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="O21" s="7"/>
+      <c r="P21" s="7"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>28</v>
       </c>
@@ -1129,8 +1502,18 @@
       </c>
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K22" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="O22" s="3"/>
+      <c r="P22" s="3"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>29</v>
       </c>
@@ -1149,8 +1532,18 @@
       </c>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>30</v>
       </c>
@@ -1169,8 +1562,18 @@
       </c>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O24" s="1"/>
+      <c r="P24" s="1"/>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>31</v>
       </c>
@@ -1189,8 +1592,18 @@
       </c>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O25" s="1"/>
+      <c r="P25" s="1"/>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>32</v>
       </c>
@@ -1209,8 +1622,18 @@
       </c>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O26" s="1"/>
+      <c r="P26" s="1"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>33</v>
       </c>
@@ -1233,8 +1656,18 @@
       </c>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K27" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L27" s="1"/>
+      <c r="M27" s="1"/>
+      <c r="N27" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O27" s="1"/>
+      <c r="P27" s="1"/>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>34</v>
       </c>
@@ -1253,8 +1686,18 @@
       </c>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
+      <c r="N28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O28" s="1"/>
+      <c r="P28" s="1"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>35</v>
       </c>
@@ -1273,8 +1716,18 @@
       </c>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K29" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
+      <c r="N29" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O29" s="1"/>
+      <c r="P29" s="1"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>36</v>
       </c>
@@ -1293,8 +1746,18 @@
       </c>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K30" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L30" s="1"/>
+      <c r="M30" s="1"/>
+      <c r="N30" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O30" s="1"/>
+      <c r="P30" s="1"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>37</v>
       </c>
@@ -1313,8 +1776,18 @@
       </c>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L31" s="1"/>
+      <c r="M31" s="1"/>
+      <c r="N31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O31" s="1"/>
+      <c r="P31" s="1"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>38</v>
       </c>
@@ -1333,8 +1806,18 @@
       </c>
       <c r="I32" s="3"/>
       <c r="J32" s="3"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K32" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="L32" s="3"/>
+      <c r="M32" s="3"/>
+      <c r="N32" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="O32" s="3"/>
+      <c r="P32" s="3"/>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>39</v>
       </c>
@@ -1353,8 +1836,18 @@
       </c>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K33" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L33" s="1"/>
+      <c r="M33" s="1"/>
+      <c r="N33" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O33" s="1"/>
+      <c r="P33" s="1"/>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>40</v>
       </c>
@@ -1377,8 +1870,18 @@
       </c>
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K34" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L34" s="1"/>
+      <c r="M34" s="1"/>
+      <c r="N34" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O34" s="1"/>
+      <c r="P34" s="1"/>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>1</v>
       </c>
@@ -1397,8 +1900,18 @@
       </c>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K35" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L35" s="1"/>
+      <c r="M35" s="1"/>
+      <c r="N35" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O35" s="1"/>
+      <c r="P35" s="1"/>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>16</v>
       </c>
@@ -1417,8 +1930,18 @@
       </c>
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K36" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L36" s="1"/>
+      <c r="M36" s="1"/>
+      <c r="N36" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O36" s="1"/>
+      <c r="P36" s="1"/>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>41</v>
       </c>
@@ -1437,8 +1960,18 @@
       </c>
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K37" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L37" s="1"/>
+      <c r="M37" s="1"/>
+      <c r="N37" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O37" s="1"/>
+      <c r="P37" s="1"/>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>42</v>
       </c>
@@ -1457,8 +1990,32 @@
       </c>
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
+      <c r="K38" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L38" s="1"/>
+      <c r="M38" s="1"/>
+      <c r="N38" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O38" s="1"/>
+      <c r="P38" s="1"/>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B41" s="5"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="5"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A41:G41"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
first of class diagrams
</commit_message>
<xml_diff>
--- a/Autres/Equilibrage/Tableau_Dépendance_Stats.xlsx
+++ b/Autres/Equilibrage/Tableau_Dépendance_Stats.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="84">
   <si>
     <t>Stress</t>
   </si>
@@ -277,6 +277,9 @@
   </si>
   <si>
     <t>_+2</t>
+  </si>
+  <si>
+    <t>Capacité(Inventaire)</t>
   </si>
 </sst>
 </file>
@@ -367,9 +370,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -377,6 +377,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -683,7 +686,7 @@
   <dimension ref="A1:P41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -866,34 +869,34 @@
       <c r="P4" s="1"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="O5" s="7"/>
-      <c r="P5" s="7"/>
+      <c r="A5" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -938,34 +941,34 @@
       <c r="P6" s="4"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="O7" s="7"/>
-      <c r="P7" s="7"/>
+      <c r="B7" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="O7" s="6"/>
+      <c r="P7" s="6"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -1002,182 +1005,182 @@
       <c r="P8" s="1"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="L9" s="8"/>
-      <c r="M9" s="8"/>
-      <c r="N9" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="O9" s="8"/>
-      <c r="P9" s="8"/>
+      <c r="B9" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="O9" s="7"/>
+      <c r="P9" s="7"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="L10" s="8"/>
-      <c r="M10" s="8"/>
-      <c r="N10" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="O10" s="8"/>
-      <c r="P10" s="8"/>
+      <c r="B10" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="7" t="s">
+      <c r="B11" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="E11" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F11" s="7" t="s">
+      <c r="E11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="G11" s="7" t="s">
+      <c r="G11" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="H11" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="I11" s="7" t="s">
+      <c r="H11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I11" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="J11" s="7" t="s">
+      <c r="J11" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="K11" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="L11" s="7" t="s">
+      <c r="K11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="L11" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="M11" s="7" t="s">
+      <c r="M11" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="N11" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="O11" s="7" t="s">
+      <c r="N11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="O11" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="P11" s="7" t="s">
+      <c r="P11" s="6" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" s="7" t="s">
+      <c r="B12" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="E12" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F12" s="7" t="s">
+      <c r="E12" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="G12" s="7" t="s">
+      <c r="G12" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="H12" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="L12" s="7"/>
-      <c r="M12" s="7"/>
-      <c r="N12" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="O12" s="7"/>
-      <c r="P12" s="7"/>
+      <c r="H12" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="O12" s="6"/>
+      <c r="P12" s="6"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="L13" s="7"/>
-      <c r="M13" s="7"/>
-      <c r="N13" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="O13" s="7"/>
-      <c r="P13" s="7"/>
+      <c r="B13" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="O13" s="6"/>
+      <c r="P13" s="6"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -1238,7 +1241,7 @@
       <c r="H15" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I15" s="6" t="s">
+      <c r="I15" s="5" t="s">
         <v>73</v>
       </c>
       <c r="J15" s="1" t="s">
@@ -1266,7 +1269,7 @@
       <c r="B16" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="5" t="s">
         <v>64</v>
       </c>
       <c r="D16" s="1" t="s">
@@ -1336,152 +1339,152 @@
       <c r="P17" s="1"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="L18" s="7"/>
-      <c r="M18" s="7"/>
-      <c r="N18" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="O18" s="7"/>
-      <c r="P18" s="7"/>
+      <c r="B18" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="L18" s="6"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="O18" s="6"/>
+      <c r="P18" s="6"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C19" s="7" t="s">
+      <c r="B19" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E19" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="I19" s="7"/>
-      <c r="J19" s="7"/>
-      <c r="K19" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="L19" s="7"/>
-      <c r="M19" s="7"/>
-      <c r="N19" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="O19" s="7"/>
-      <c r="P19" s="7"/>
+      <c r="E19" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="L19" s="6"/>
+      <c r="M19" s="6"/>
+      <c r="N19" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="O19" s="6"/>
+      <c r="P19" s="6"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C20" s="7" t="s">
+      <c r="B20" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E20" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F20" s="7" t="s">
+      <c r="E20" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F20" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="G20" s="7" t="s">
+      <c r="G20" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="H20" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="I20" s="7" t="s">
+      <c r="H20" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I20" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="J20" s="7" t="s">
+      <c r="J20" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="K20" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="L20" s="7"/>
-      <c r="M20" s="7"/>
-      <c r="N20" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="O20" s="7"/>
-      <c r="P20" s="7"/>
+      <c r="K20" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="L20" s="6"/>
+      <c r="M20" s="6"/>
+      <c r="N20" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="O20" s="6"/>
+      <c r="P20" s="6"/>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C21" s="7" t="s">
+      <c r="B21" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="D21" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E21" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F21" s="7" t="s">
+      <c r="E21" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F21" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="G21" s="7" t="s">
+      <c r="G21" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="H21" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="I21" s="7" t="s">
+      <c r="H21" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I21" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="J21" s="7" t="s">
+      <c r="J21" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="K21" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="L21" s="7"/>
-      <c r="M21" s="7"/>
-      <c r="N21" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="O21" s="7"/>
-      <c r="P21" s="7"/>
+      <c r="K21" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="L21" s="6"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="O21" s="6"/>
+      <c r="P21" s="6"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
@@ -2002,15 +2005,15 @@
       <c r="P38" s="1"/>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A41" s="5" t="s">
+      <c r="A41" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="B41" s="5"/>
-      <c r="C41" s="5"/>
-      <c r="D41" s="5"/>
-      <c r="E41" s="5"/>
-      <c r="F41" s="5"/>
-      <c r="G41" s="5"/>
+      <c r="B41" s="8"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="8"/>
+      <c r="E41" s="8"/>
+      <c r="F41" s="8"/>
+      <c r="G41" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
continuing of mcv creation + update manuel
</commit_message>
<xml_diff>
--- a/Autres/Equilibrage/Tableau_Dépendance_Stats.xlsx
+++ b/Autres/Equilibrage/Tableau_Dépendance_Stats.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="103">
   <si>
     <t>Stress</t>
   </si>
@@ -103,33 +103,6 @@
   </si>
   <si>
     <t>Habiletés des personnages</t>
-  </si>
-  <si>
-    <t>Chimiste</t>
-  </si>
-  <si>
-    <t>Policier</t>
-  </si>
-  <si>
-    <t>Politicien</t>
-  </si>
-  <si>
-    <t>Eletricien</t>
-  </si>
-  <si>
-    <t>Cambrioleur</t>
-  </si>
-  <si>
-    <t>Leadeur</t>
-  </si>
-  <si>
-    <t>Bricoleur</t>
-  </si>
-  <si>
-    <t>Athlète</t>
-  </si>
-  <si>
-    <t>Chasseur</t>
   </si>
   <si>
     <t>Caractéristiques des zombis</t>
@@ -280,6 +253,90 @@
   </si>
   <si>
     <t>Capacité(Inventaire)</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>Infos Médicaments</t>
+  </si>
+  <si>
+    <t>Chimie</t>
+  </si>
+  <si>
+    <t>Créer bombe</t>
+  </si>
+  <si>
+    <t>Créer Molotov</t>
+  </si>
+  <si>
+    <t>Gestion des foules</t>
+  </si>
+  <si>
+    <t>Utiliser arme à feu</t>
+  </si>
+  <si>
+    <t>Charisme</t>
+  </si>
+  <si>
+    <t>Eletricité</t>
+  </si>
+  <si>
+    <t>Cambriolage</t>
+  </si>
+  <si>
+    <t>Gestion de groupe</t>
+  </si>
+  <si>
+    <t>Bricoler</t>
+  </si>
+  <si>
+    <t>Athlétisme</t>
+  </si>
+  <si>
+    <t>Chasse</t>
+  </si>
+  <si>
+    <t>ET(x) signifie que le bonus de poids x est appliqué sur l'entourage du joueur. C'est une application temporaire.</t>
+  </si>
+  <si>
+    <t>ED(x, A) signifie que le bonus de poids x est appliqué sur l'entourage du joueur. C'est une application définitive qui arrive lors de l'action A.</t>
+  </si>
+  <si>
+    <t>ET(_-10)</t>
+  </si>
+  <si>
+    <t>_-= 0,2</t>
+  </si>
+  <si>
+    <t>BonusSM</t>
+  </si>
+  <si>
+    <t>ET(_+0,2)</t>
+  </si>
+  <si>
+    <t>Utiliser objet électrique</t>
+  </si>
+  <si>
+    <t>Crocheter Serrure</t>
+  </si>
+  <si>
+    <t>Pister cible</t>
+  </si>
+  <si>
+    <t>Conseil bon sens</t>
+  </si>
+  <si>
+    <t>ET(_+1)</t>
+  </si>
+  <si>
+    <t>Mélomanie</t>
+  </si>
+  <si>
+    <t>_-1</t>
+  </si>
+  <si>
+    <t>Bonus Fatigue</t>
   </si>
 </sst>
 </file>
@@ -356,7 +413,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -377,6 +434,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -683,24 +743,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P41"/>
+  <dimension ref="A1:P44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="3.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="2.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="2.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="2.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9" style="2" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
@@ -737,17 +797,17 @@
       </c>
       <c r="K1" s="1"/>
       <c r="L1" s="1" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="N1" s="1"/>
       <c r="O1" s="1" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
@@ -791,25 +851,25 @@
         <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>7</v>
@@ -837,7 +897,7 @@
         <v>5</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>7</v>
@@ -846,7 +906,7 @@
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>7</v>
@@ -855,7 +915,7 @@
         <v>5</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>7</v>
@@ -870,7 +930,7 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>4</v>
@@ -915,10 +975,10 @@
         <v>7</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>7</v>
@@ -981,7 +1041,7 @@
         <v>1</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>7</v>
@@ -1072,46 +1132,46 @@
         <v>4</v>
       </c>
       <c r="C11" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="J11" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="D11" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F11" s="6" t="s">
+      <c r="K11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="L11" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="G11" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="H11" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="I11" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="J11" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="K11" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="L11" s="6" t="s">
-        <v>61</v>
-      </c>
       <c r="M11" s="6" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="N11" s="6" t="s">
         <v>7</v>
       </c>
       <c r="O11" s="6" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="P11" s="6" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
@@ -1122,19 +1182,19 @@
         <v>4</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>7</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="H12" s="6" t="s">
         <v>7</v>
@@ -1154,7 +1214,7 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>4</v>
@@ -1190,7 +1250,7 @@
         <v>4</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>25</v>
@@ -1224,37 +1284,37 @@
         <v>4</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>7</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="K15" s="1" t="s">
         <v>7</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="N15" s="1" t="s">
         <v>7</v>
@@ -1270,19 +1330,19 @@
         <v>4</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>7</v>
@@ -1308,19 +1368,19 @@
         <v>4</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>7</v>
@@ -1376,7 +1436,7 @@
         <v>4</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>21</v>
@@ -1410,7 +1470,7 @@
         <v>4</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>21</v>
@@ -1419,16 +1479,16 @@
         <v>7</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="H20" s="6" t="s">
         <v>7</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="J20" s="6" t="s">
         <v>19</v>
@@ -1452,7 +1512,7 @@
         <v>4</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>21</v>
@@ -1461,7 +1521,7 @@
         <v>7</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="G21" s="6" t="s">
         <v>20</v>
@@ -1470,10 +1530,10 @@
         <v>7</v>
       </c>
       <c r="I21" s="6" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="K21" s="6" t="s">
         <v>7</v>
@@ -1518,23 +1578,35 @@
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>29</v>
+        <v>77</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
+      <c r="C23" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>76</v>
+      </c>
       <c r="E23" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
+      <c r="F23" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="H23" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
+      <c r="I23" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>79</v>
+      </c>
       <c r="K23" s="1" t="s">
         <v>7</v>
       </c>
@@ -1548,18 +1620,26 @@
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>30</v>
+        <v>80</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
+      <c r="C24" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>81</v>
+      </c>
       <c r="E24" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
+      <c r="F24" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="H24" s="1" t="s">
         <v>7</v>
       </c>
@@ -1578,23 +1658,35 @@
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>31</v>
+        <v>82</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
+      <c r="C25" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="E25" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
+      <c r="F25" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>93</v>
+      </c>
       <c r="H25" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
+      <c r="I25" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="K25" s="1" t="s">
         <v>7</v>
       </c>
@@ -1608,13 +1700,17 @@
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>32</v>
+        <v>83</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
+      <c r="C26" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>95</v>
+      </c>
       <c r="E26" s="1" t="s">
         <v>7</v>
       </c>
@@ -1638,7 +1734,7 @@
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>33</v>
+        <v>84</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>4</v>
@@ -1647,13 +1743,17 @@
         <v>0.05</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
+      <c r="F27" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>96</v>
+      </c>
       <c r="H27" s="1" t="s">
         <v>7</v>
       </c>
@@ -1672,18 +1772,26 @@
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>34</v>
+        <v>85</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
+      <c r="C28" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>98</v>
+      </c>
       <c r="E28" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
+      <c r="F28" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="H28" s="1" t="s">
         <v>7</v>
       </c>
@@ -1702,13 +1810,17 @@
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>35</v>
+        <v>86</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
+      <c r="C29" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>86</v>
+      </c>
       <c r="E29" s="1" t="s">
         <v>7</v>
       </c>
@@ -1730,15 +1842,19 @@
       <c r="O29" s="1"/>
       <c r="P29" s="1"/>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>36</v>
+        <v>100</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
+      <c r="C30" s="1">
+        <v>3</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="E30" s="1" t="s">
         <v>7</v>
       </c>
@@ -1749,26 +1865,26 @@
       </c>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
-      <c r="K30" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="K30" s="1"/>
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
-      <c r="N30" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="N30" s="1"/>
       <c r="O30" s="1"/>
       <c r="P30" s="1"/>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>37</v>
+        <v>87</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
+      <c r="C31" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>102</v>
+      </c>
       <c r="E31" s="1" t="s">
         <v>7</v>
       </c>
@@ -1791,78 +1907,78 @@
       <c r="P31" s="1"/>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F32" s="3"/>
-      <c r="G32" s="3"/>
-      <c r="H32" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I32" s="3"/>
-      <c r="J32" s="3"/>
-      <c r="K32" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="L32" s="3"/>
-      <c r="M32" s="3"/>
-      <c r="N32" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="O32" s="3"/>
-      <c r="P32" s="3"/>
+      <c r="A32" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L32" s="1"/>
+      <c r="M32" s="1"/>
+      <c r="N32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O32" s="1"/>
+      <c r="P32" s="1"/>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
-      <c r="H33" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I33" s="1"/>
-      <c r="J33" s="1"/>
-      <c r="K33" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="L33" s="1"/>
-      <c r="M33" s="1"/>
-      <c r="N33" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="O33" s="1"/>
-      <c r="P33" s="1"/>
+      <c r="A33" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I33" s="3"/>
+      <c r="J33" s="3"/>
+      <c r="K33" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="L33" s="3"/>
+      <c r="M33" s="3"/>
+      <c r="N33" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="O33" s="3"/>
+      <c r="P33" s="3"/>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C34" s="1">
-        <v>1</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>54</v>
-      </c>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
       <c r="E34" s="1" t="s">
         <v>7</v>
       </c>
@@ -1886,13 +2002,17 @@
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C35" s="1">
         <v>1</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
+      <c r="D35" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="E35" s="1" t="s">
         <v>7</v>
       </c>
@@ -1916,7 +2036,7 @@
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>4</v>
@@ -1946,7 +2066,7 @@
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>4</v>
@@ -1976,7 +2096,7 @@
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>4</v>
@@ -2004,20 +2124,92 @@
       <c r="O38" s="1"/>
       <c r="P38" s="1"/>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A41" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="B41" s="8"/>
-      <c r="C41" s="8"/>
-      <c r="D41" s="8"/>
-      <c r="E41" s="8"/>
-      <c r="F41" s="8"/>
-      <c r="G41" s="8"/>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I39" s="1"/>
+      <c r="J39" s="1"/>
+      <c r="K39" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L39" s="1"/>
+      <c r="M39" s="1"/>
+      <c r="N39" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O39" s="1"/>
+      <c r="P39" s="1"/>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A42" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="B42" s="9"/>
+      <c r="C42" s="9"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="9"/>
+      <c r="F42" s="9"/>
+      <c r="G42" s="9"/>
+      <c r="H42" s="9"/>
+      <c r="I42" s="9"/>
+      <c r="J42" s="9"/>
+      <c r="K42" s="9"/>
+      <c r="L42" s="9"/>
+      <c r="M42" s="9"/>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A43" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="B43" s="9"/>
+      <c r="C43" s="9"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="9"/>
+      <c r="F43" s="9"/>
+      <c r="G43" s="9"/>
+      <c r="H43" s="9"/>
+      <c r="I43" s="9"/>
+      <c r="J43" s="9"/>
+      <c r="K43" s="9"/>
+      <c r="L43" s="9"/>
+      <c r="M43" s="9"/>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A44" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="B44" s="9"/>
+      <c r="C44" s="9"/>
+      <c r="D44" s="9"/>
+      <c r="E44" s="9"/>
+      <c r="F44" s="9"/>
+      <c r="G44" s="9"/>
+      <c r="H44" s="9"/>
+      <c r="I44" s="9"/>
+      <c r="J44" s="9"/>
+      <c r="K44" s="9"/>
+      <c r="L44" s="9"/>
+      <c r="M44" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A41:G41"/>
+  <mergeCells count="3">
+    <mergeCell ref="A43:M43"/>
+    <mergeCell ref="A42:M42"/>
+    <mergeCell ref="A44:M44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>